<commit_message>
Eliminación de recursos 11_15
Eliminación de recursos 11_15
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion15/Escaleta_CN_11_15_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion15/Escaleta_CN_11_15_CO.xlsx
@@ -860,7 +860,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,6 +939,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -996,7 +1002,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1069,22 +1075,57 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1126,44 +1167,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1171,6 +1190,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1472,8 +1496,8 @@
   <dimension ref="A1:U297"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I45" sqref="I45"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,94 +1525,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="29" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="69"/>
+      <c r="O1" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="59" t="s">
+      <c r="T1" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="57" t="s">
+      <c r="U1" s="51" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="49"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="66"/>
+      <c r="L2" s="64"/>
       <c r="M2" s="30" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="58"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -1608,7 +1632,7 @@
       <c r="G3" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="H3" s="39">
+      <c r="H3" s="38">
         <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
@@ -1680,62 +1704,62 @@
       <c r="T4" s="28"/>
       <c r="U4" s="26"/>
     </row>
-    <row r="5" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+    <row r="5" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65" t="s">
+      <c r="F5" s="41"/>
+      <c r="G5" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="42">
         <v>2</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="K5" s="67" t="s">
+      <c r="K5" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="N5" s="67"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65" t="s">
+      <c r="N5" s="43"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="65">
+      <c r="Q5" s="41">
         <v>6</v>
       </c>
-      <c r="R5" s="65" t="s">
+      <c r="R5" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S5" s="65" t="s">
+      <c r="S5" s="41" t="s">
         <v>171</v>
       </c>
-      <c r="T5" s="65" t="s">
+      <c r="T5" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="U5" s="65" t="s">
+      <c r="U5" s="41" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1759,7 +1783,7 @@
         <v>127</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="39"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="5"/>
       <c r="J6" s="17"/>
       <c r="K6" s="7"/>
@@ -1774,64 +1798,64 @@
       <c r="T6" s="12"/>
       <c r="U6" s="10"/>
     </row>
-    <row r="7" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+    <row r="7" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="42">
         <v>3</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="65" t="s">
+      <c r="J7" s="41" t="s">
         <v>248</v>
       </c>
-      <c r="K7" s="67" t="s">
+      <c r="K7" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L7" s="67" t="s">
+      <c r="L7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67" t="s">
+      <c r="M7" s="43"/>
+      <c r="N7" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="O7" s="65"/>
-      <c r="P7" s="65" t="s">
+      <c r="O7" s="41"/>
+      <c r="P7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="65">
+      <c r="Q7" s="41">
         <v>6</v>
       </c>
-      <c r="R7" s="65" t="s">
+      <c r="R7" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S7" s="65" t="s">
+      <c r="S7" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="T7" s="65" t="s">
+      <c r="T7" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="U7" s="65" t="s">
+      <c r="U7" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1855,7 +1879,7 @@
         <v>130</v>
       </c>
       <c r="G8" s="16"/>
-      <c r="H8" s="39"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="5"/>
       <c r="J8" s="17"/>
       <c r="K8" s="7"/>
@@ -1890,7 +1914,7 @@
         <v>131</v>
       </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="39"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="5"/>
       <c r="J9" s="17"/>
       <c r="K9" s="7"/>
@@ -1925,7 +1949,7 @@
         <v>132</v>
       </c>
       <c r="G10" s="16"/>
-      <c r="H10" s="39"/>
+      <c r="H10" s="38"/>
       <c r="I10" s="5"/>
       <c r="J10" s="17"/>
       <c r="K10" s="7"/>
@@ -1960,7 +1984,7 @@
         <v>134</v>
       </c>
       <c r="G11" s="16"/>
-      <c r="H11" s="39"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="5"/>
       <c r="J11" s="17"/>
       <c r="K11" s="7"/>
@@ -1995,7 +2019,7 @@
         <v>135</v>
       </c>
       <c r="G12" s="16"/>
-      <c r="H12" s="39"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="5"/>
       <c r="J12" s="17"/>
       <c r="K12" s="7"/>
@@ -2030,7 +2054,7 @@
         <v>137</v>
       </c>
       <c r="G13" s="16"/>
-      <c r="H13" s="39"/>
+      <c r="H13" s="38"/>
       <c r="I13" s="5"/>
       <c r="J13" s="17"/>
       <c r="K13" s="7"/>
@@ -2065,7 +2089,7 @@
         <v>138</v>
       </c>
       <c r="G14" s="16"/>
-      <c r="H14" s="39"/>
+      <c r="H14" s="38"/>
       <c r="I14" s="5"/>
       <c r="J14" s="17"/>
       <c r="K14" s="7"/>
@@ -2100,7 +2124,7 @@
         <v>139</v>
       </c>
       <c r="G15" s="16"/>
-      <c r="H15" s="39"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="5"/>
       <c r="J15" s="17"/>
       <c r="K15" s="7"/>
@@ -2135,7 +2159,7 @@
         <v>141</v>
       </c>
       <c r="G16" s="16"/>
-      <c r="H16" s="39"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="5"/>
       <c r="J16" s="17"/>
       <c r="K16" s="7"/>
@@ -2170,7 +2194,7 @@
         <v>142</v>
       </c>
       <c r="G17" s="16"/>
-      <c r="H17" s="39"/>
+      <c r="H17" s="38"/>
       <c r="I17" s="5"/>
       <c r="J17" s="17"/>
       <c r="K17" s="7"/>
@@ -2207,7 +2231,7 @@
       <c r="G18" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="38">
         <v>4</v>
       </c>
       <c r="I18" s="5" t="s">
@@ -2246,64 +2270,64 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="63" t="s">
+    <row r="19" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="63" t="s">
+      <c r="B19" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="63" t="s">
+      <c r="C19" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E19" s="65" t="s">
+      <c r="E19" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="F19" s="65" t="s">
+      <c r="F19" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="65" t="s">
+      <c r="G19" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="H19" s="66">
+      <c r="H19" s="42">
         <v>5</v>
       </c>
-      <c r="I19" s="67" t="s">
+      <c r="I19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="65" t="s">
+      <c r="J19" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="K19" s="67" t="s">
+      <c r="K19" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="67" t="s">
+      <c r="L19" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="67"/>
-      <c r="N19" s="67" t="s">
+      <c r="M19" s="43"/>
+      <c r="N19" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65" t="s">
+      <c r="O19" s="41"/>
+      <c r="P19" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="Q19" s="65">
+      <c r="Q19" s="41">
         <v>6</v>
       </c>
-      <c r="R19" s="65" t="s">
+      <c r="R19" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S19" s="65" t="s">
+      <c r="S19" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="T19" s="65" t="s">
+      <c r="T19" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="U19" s="65" t="s">
+      <c r="U19" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2325,7 +2349,7 @@
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="16"/>
-      <c r="H20" s="39"/>
+      <c r="H20" s="38"/>
       <c r="I20" s="5"/>
       <c r="J20" s="17"/>
       <c r="K20" s="7"/>
@@ -2358,7 +2382,7 @@
       </c>
       <c r="F21" s="9"/>
       <c r="G21" s="16"/>
-      <c r="H21" s="39"/>
+      <c r="H21" s="38"/>
       <c r="I21" s="5"/>
       <c r="J21" s="17"/>
       <c r="K21" s="7"/>
@@ -2373,62 +2397,62 @@
       <c r="T21" s="12"/>
       <c r="U21" s="10"/>
     </row>
-    <row r="22" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="63" t="s">
+    <row r="22" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="63" t="s">
+      <c r="C22" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="64" t="s">
+      <c r="D22" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="65" t="s">
+      <c r="E22" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65" t="s">
+      <c r="F22" s="41"/>
+      <c r="G22" s="41" t="s">
         <v>197</v>
       </c>
-      <c r="H22" s="66">
+      <c r="H22" s="42">
         <v>6</v>
       </c>
-      <c r="I22" s="67" t="s">
+      <c r="I22" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="65" t="s">
+      <c r="J22" s="41" t="s">
         <v>254</v>
       </c>
-      <c r="K22" s="67" t="s">
+      <c r="K22" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="67" t="s">
+      <c r="L22" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="M22" s="67" t="s">
+      <c r="M22" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="N22" s="67"/>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65" t="s">
+      <c r="N22" s="43"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="65">
+      <c r="Q22" s="41">
         <v>6</v>
       </c>
-      <c r="R22" s="65" t="s">
+      <c r="R22" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="S22" s="65" t="s">
+      <c r="S22" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="T22" s="65" t="s">
+      <c r="T22" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="U22" s="65" t="s">
+      <c r="U22" s="41" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2452,7 +2476,7 @@
       <c r="G23" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="38">
         <v>7</v>
       </c>
       <c r="I23" s="5" t="s">
@@ -2509,7 +2533,7 @@
       <c r="G24" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="H24" s="39">
+      <c r="H24" s="38">
         <v>8</v>
       </c>
       <c r="I24" s="5" t="s">
@@ -2566,7 +2590,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="39"/>
+      <c r="H25" s="38"/>
       <c r="I25" s="5"/>
       <c r="J25" s="17"/>
       <c r="K25" s="7"/>
@@ -2599,7 +2623,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="16"/>
-      <c r="H26" s="39"/>
+      <c r="H26" s="38"/>
       <c r="I26" s="5"/>
       <c r="J26" s="17"/>
       <c r="K26" s="7"/>
@@ -2632,7 +2656,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="39"/>
+      <c r="H27" s="38"/>
       <c r="I27" s="5"/>
       <c r="J27" s="17"/>
       <c r="K27" s="7"/>
@@ -2667,7 +2691,7 @@
       <c r="G28" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="H28" s="39">
+      <c r="H28" s="38">
         <v>9</v>
       </c>
       <c r="I28" s="5" t="s">
@@ -2706,62 +2730,62 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="63" t="s">
+    <row r="29" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="69" t="s">
+      <c r="D29" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E29" s="70" t="s">
+      <c r="E29" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65" t="s">
+      <c r="F29" s="41"/>
+      <c r="G29" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="H29" s="66">
+      <c r="H29" s="42">
         <v>10</v>
       </c>
-      <c r="I29" s="67" t="s">
+      <c r="I29" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="65" t="s">
+      <c r="J29" s="41" t="s">
         <v>229</v>
       </c>
-      <c r="K29" s="67" t="s">
+      <c r="K29" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="67" t="s">
+      <c r="L29" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="67"/>
-      <c r="N29" s="67" t="s">
+      <c r="M29" s="43"/>
+      <c r="N29" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="O29" s="65"/>
-      <c r="P29" s="65" t="s">
+      <c r="O29" s="41"/>
+      <c r="P29" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="Q29" s="65">
+      <c r="Q29" s="41">
         <v>6</v>
       </c>
-      <c r="R29" s="65" t="s">
+      <c r="R29" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S29" s="65" t="s">
+      <c r="S29" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="T29" s="65" t="s">
+      <c r="T29" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="U29" s="65" t="s">
+      <c r="U29" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2785,7 +2809,7 @@
         <v>153</v>
       </c>
       <c r="G30" s="16"/>
-      <c r="H30" s="39"/>
+      <c r="H30" s="38"/>
       <c r="I30" s="5"/>
       <c r="J30" s="17"/>
       <c r="K30" s="7"/>
@@ -2800,64 +2824,64 @@
       <c r="T30" s="12"/>
       <c r="U30" s="10"/>
     </row>
-    <row r="31" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="63" t="s">
+    <row r="31" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="63" t="s">
+      <c r="B31" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="69" t="s">
+      <c r="D31" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="E31" s="71" t="s">
+      <c r="E31" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="F31" s="65" t="s">
+      <c r="F31" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="G31" s="65" t="s">
+      <c r="G31" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="H31" s="66">
+      <c r="H31" s="42">
         <v>11</v>
       </c>
-      <c r="I31" s="67" t="s">
+      <c r="I31" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="65" t="s">
+      <c r="J31" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="K31" s="67" t="s">
+      <c r="K31" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="67" t="s">
+      <c r="L31" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="67"/>
-      <c r="N31" s="67" t="s">
+      <c r="M31" s="43"/>
+      <c r="N31" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="O31" s="65"/>
-      <c r="P31" s="65" t="s">
+      <c r="O31" s="41"/>
+      <c r="P31" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q31" s="65">
+      <c r="Q31" s="41">
         <v>6</v>
       </c>
-      <c r="R31" s="65" t="s">
+      <c r="R31" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S31" s="65" t="s">
+      <c r="S31" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="T31" s="65" t="s">
+      <c r="T31" s="41" t="s">
         <v>228</v>
       </c>
-      <c r="U31" s="65" t="s">
+      <c r="U31" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2883,7 +2907,7 @@
       <c r="G32" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="H32" s="39">
+      <c r="H32" s="38">
         <v>12</v>
       </c>
       <c r="I32" s="5" t="s">
@@ -2942,7 +2966,7 @@
       <c r="G33" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="38">
         <v>13</v>
       </c>
       <c r="I33" s="5" t="s">
@@ -3001,7 +3025,7 @@
       <c r="G34" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="H34" s="39">
+      <c r="H34" s="38">
         <v>14</v>
       </c>
       <c r="I34" s="5" t="s">
@@ -3060,7 +3084,7 @@
         <v>156</v>
       </c>
       <c r="G35" s="16"/>
-      <c r="H35" s="39"/>
+      <c r="H35" s="38"/>
       <c r="I35" s="5"/>
       <c r="J35" s="17"/>
       <c r="K35" s="7"/>
@@ -3097,7 +3121,7 @@
       <c r="G36" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="H36" s="39">
+      <c r="H36" s="38">
         <v>15</v>
       </c>
       <c r="I36" s="5" t="s">
@@ -3156,7 +3180,7 @@
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="39"/>
+      <c r="H37" s="38"/>
       <c r="I37" s="5"/>
       <c r="J37" s="17"/>
       <c r="K37" s="7"/>
@@ -3191,7 +3215,7 @@
       <c r="G38" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="38">
         <v>16</v>
       </c>
       <c r="I38" s="5" t="s">
@@ -3248,7 +3272,7 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="16"/>
-      <c r="H39" s="39"/>
+      <c r="H39" s="38"/>
       <c r="I39" s="5"/>
       <c r="J39" s="17"/>
       <c r="K39" s="7"/>
@@ -3263,180 +3287,180 @@
       <c r="T39" s="12"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="63" t="s">
+    <row r="40" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C40" s="63" t="s">
+      <c r="C40" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="65" t="s">
+      <c r="D40" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="E40" s="71" t="s">
+      <c r="E40" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65" t="s">
+      <c r="F40" s="41"/>
+      <c r="G40" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="H40" s="66">
+      <c r="H40" s="42">
         <v>17</v>
       </c>
-      <c r="I40" s="67" t="s">
+      <c r="I40" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="J40" s="65" t="s">
+      <c r="J40" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="K40" s="67" t="s">
+      <c r="K40" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="67" t="s">
+      <c r="L40" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="M40" s="67"/>
-      <c r="N40" s="67"/>
-      <c r="O40" s="72" t="s">
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="P40" s="65" t="s">
+      <c r="P40" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q40" s="65">
+      <c r="Q40" s="41">
         <v>6</v>
       </c>
-      <c r="R40" s="65" t="s">
+      <c r="R40" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="S40" s="65" t="s">
+      <c r="S40" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="T40" s="65" t="s">
+      <c r="T40" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="U40" s="65" t="s">
+      <c r="U40" s="41" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+    <row r="41" spans="1:21" s="76" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="16" t="s">
+      <c r="F41" s="73"/>
+      <c r="G41" s="73" t="s">
         <v>230</v>
       </c>
-      <c r="H41" s="39">
+      <c r="H41" s="74">
         <v>18</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J41" s="17" t="s">
+      <c r="J41" s="73" t="s">
         <v>231</v>
       </c>
-      <c r="K41" s="7" t="s">
+      <c r="K41" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="L41" s="6" t="s">
+      <c r="L41" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8" t="s">
+      <c r="M41" s="75"/>
+      <c r="N41" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="O41" s="37"/>
-      <c r="P41" s="9" t="s">
+      <c r="O41" s="79"/>
+      <c r="P41" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="Q41" s="10">
+      <c r="Q41" s="73">
         <v>6</v>
       </c>
-      <c r="R41" s="11" t="s">
+      <c r="R41" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="S41" s="10" t="s">
+      <c r="S41" s="73" t="s">
         <v>178</v>
       </c>
-      <c r="T41" s="12" t="s">
+      <c r="T41" s="73" t="s">
         <v>233</v>
       </c>
-      <c r="U41" s="10" t="s">
+      <c r="U41" s="73" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="63" t="s">
+    <row r="42" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="65" t="s">
+      <c r="D42" s="41" t="s">
         <v>154</v>
       </c>
-      <c r="E42" s="71" t="s">
+      <c r="E42" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65" t="s">
+      <c r="F42" s="41"/>
+      <c r="G42" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="H42" s="66">
+      <c r="H42" s="42">
         <v>19</v>
       </c>
-      <c r="I42" s="67" t="s">
+      <c r="I42" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J42" s="65" t="s">
+      <c r="J42" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="K42" s="67" t="s">
+      <c r="K42" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L42" s="67" t="s">
+      <c r="L42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M42" s="67"/>
-      <c r="N42" s="67" t="s">
+      <c r="M42" s="43"/>
+      <c r="N42" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="O42" s="72"/>
-      <c r="P42" s="65" t="s">
+      <c r="O42" s="48"/>
+      <c r="P42" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q42" s="65">
+      <c r="Q42" s="41">
         <v>6</v>
       </c>
-      <c r="R42" s="65" t="s">
+      <c r="R42" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S42" s="65" t="s">
+      <c r="S42" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="T42" s="65" t="s">
+      <c r="T42" s="41" t="s">
         <v>236</v>
       </c>
-      <c r="U42" s="65" t="s">
+      <c r="U42" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3460,7 +3484,7 @@
       <c r="G43" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="H43" s="39">
+      <c r="H43" s="38">
         <v>20</v>
       </c>
       <c r="I43" s="5" t="s">
@@ -3499,117 +3523,117 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+    <row r="44" spans="1:21" s="76" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="16" t="s">
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="H44" s="39">
+      <c r="H44" s="74">
         <v>21</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="K44" s="7" t="s">
+      <c r="K44" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="L44" s="6" t="s">
+      <c r="L44" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8" t="s">
+      <c r="M44" s="75"/>
+      <c r="N44" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9" t="s">
+      <c r="O44" s="73"/>
+      <c r="P44" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="Q44" s="10">
+      <c r="Q44" s="73">
         <v>6</v>
       </c>
-      <c r="R44" s="11" t="s">
+      <c r="R44" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="S44" s="10" t="s">
+      <c r="S44" s="73" t="s">
         <v>178</v>
       </c>
-      <c r="T44" s="12" t="s">
+      <c r="T44" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="U44" s="10" t="s">
+      <c r="U44" s="73" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
+    <row r="45" spans="1:21" s="76" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="16" t="s">
+      <c r="E45" s="73"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="73" t="s">
         <v>246</v>
       </c>
-      <c r="H45" s="39">
+      <c r="H45" s="74">
         <v>22</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="J45" s="38" t="s">
+      <c r="J45" s="77" t="s">
         <v>247</v>
       </c>
-      <c r="K45" s="7" t="s">
+      <c r="K45" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="L45" s="6" t="s">
+      <c r="L45" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8" t="s">
+      <c r="M45" s="75"/>
+      <c r="N45" s="75" t="s">
         <v>120</v>
       </c>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9" t="s">
+      <c r="O45" s="73"/>
+      <c r="P45" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="Q45" s="10">
+      <c r="Q45" s="73">
         <v>6</v>
       </c>
-      <c r="R45" s="11" t="s">
+      <c r="R45" s="73" t="s">
         <v>170</v>
       </c>
-      <c r="S45" s="10" t="s">
+      <c r="S45" s="73" t="s">
         <v>178</v>
       </c>
-      <c r="T45" s="12" t="s">
+      <c r="T45" s="73" t="s">
         <v>207</v>
       </c>
-      <c r="U45" s="10" t="s">
+      <c r="U45" s="73" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3631,7 +3655,7 @@
       <c r="G46" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="H46" s="39">
+      <c r="H46" s="38">
         <v>23</v>
       </c>
       <c r="I46" s="5" t="s">
@@ -3670,60 +3694,60 @@
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:21" s="68" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="63" t="s">
+    <row r="47" spans="1:21" s="44" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="63" t="s">
+      <c r="B47" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C47" s="63" t="s">
+      <c r="C47" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="65" t="s">
+      <c r="D47" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="E47" s="65"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="65" t="s">
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="H47" s="66">
+      <c r="H47" s="42">
         <v>24</v>
       </c>
-      <c r="I47" s="67" t="s">
+      <c r="I47" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="J47" s="65" t="s">
+      <c r="J47" s="41" t="s">
         <v>252</v>
       </c>
-      <c r="K47" s="67" t="s">
+      <c r="K47" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="L47" s="67" t="s">
+      <c r="L47" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="M47" s="67"/>
-      <c r="N47" s="67" t="s">
+      <c r="M47" s="43"/>
+      <c r="N47" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="O47" s="65"/>
-      <c r="P47" s="65" t="s">
+      <c r="O47" s="41"/>
+      <c r="P47" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="Q47" s="65">
+      <c r="Q47" s="41">
         <v>6</v>
       </c>
-      <c r="R47" s="65" t="s">
+      <c r="R47" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="S47" s="65" t="s">
+      <c r="S47" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="T47" s="65" t="s">
+      <c r="T47" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="U47" s="65" t="s">
+      <c r="U47" s="41" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3745,7 +3769,7 @@
       <c r="G48" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H48" s="39">
+      <c r="H48" s="38">
         <v>25</v>
       </c>
       <c r="I48" s="5" t="s">
@@ -3790,7 +3814,7 @@
       <c r="G49" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="H49" s="39">
+      <c r="H49" s="38">
         <v>26</v>
       </c>
       <c r="I49" s="5" t="s">
@@ -3847,7 +3871,7 @@
       <c r="G50" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="H50" s="39">
+      <c r="H50" s="38">
         <v>27</v>
       </c>
       <c r="I50" s="5" t="s">
@@ -5008,12 +5032,6 @@
     <row r="297" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -5028,6 +5046,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O40" r:id="rId1"/>

</xml_diff>